<commit_message>
Update generated Excel file
</commit_message>
<xml_diff>
--- a/dbc_signals.xlsx
+++ b/dbc_signals.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="33" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="8" customWidth="1" min="6" max="6"/>
     <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="5" customWidth="1" min="8" max="8"/>
-    <col width="5" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="7" customWidth="1" min="9" max="9"/>
     <col width="6" customWidth="1" min="10" max="10"/>
-    <col width="129" customWidth="1" min="11" max="11"/>
+    <col width="130" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -824,6 +824,382 @@
         </is>
       </c>
       <c r="K10" s="3" t="inlineStr"/>
+    </row>
+    <row r="11"/>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Message: dir_actuator_feedback</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>ID: 0x2968</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Sender(s): AK10_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Signal Name</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>Start Bit</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Length (bits)</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>Byte Order</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>Signed</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>Factor</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Offset</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="I13" s="2" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>Choices</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>-32000</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>32000</v>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>º</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Speed</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>-32000</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>32000</v>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>RPM</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3" t="n"/>
+      <c r="I16" s="3" t="n"/>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Temperature</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>-20</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>127</v>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>º</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Error_codes</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J18" s="3" t="n"/>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>0=No Fault, 1=Motor Over-temperature, 2=Over-current, 3=Over-voltage, 4=Encode Fault, 5=Mosfet Over-temperature, 6=Motor Lock-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Message: dir_act_possition_loop</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>ID: 0x468</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Sender(s): JETSON</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Signal Name</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>Start Bit</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>Length (bits)</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>Byte Order</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>Signed</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>Factor</t>
+        </is>
+      </c>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>Offset</t>
+        </is>
+      </c>
+      <c r="H21" s="2" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="I21" s="2" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J21" s="2" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="inlineStr">
+        <is>
+          <t>Choices</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>RPM</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3" t="n"/>
+      <c r="I22" s="3" t="n"/>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>RPM</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>